<commit_message>
Cleaning up version 1
</commit_message>
<xml_diff>
--- a/Company Prison Labor Search.xlsx
+++ b/Company Prison Labor Search.xlsx
@@ -16,6 +16,12 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
+    <t>Starbucks</t>
+  </si>
+  <si>
+    <t>43600</t>
+  </si>
+  <si>
     <t>Mcdonald's</t>
   </si>
   <si>
@@ -26,12 +32,6 @@
   </si>
   <si>
     <t>14700</t>
-  </si>
-  <si>
-    <t>Starbucks</t>
-  </si>
-  <si>
-    <t>9310</t>
   </si>
   <si>
     <t>Burger King</t>

</xml_diff>